<commit_message>
Started Soil Moisture Analysis
</commit_message>
<xml_diff>
--- a/ExtraDetails.xlsx
+++ b/ExtraDetails.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Bayer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{707E054D-9E61-44BB-885E-380187660348}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB0E3E9D-A2EA-457B-B741-8C2961469F4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{3892B6D0-7AE6-4835-A97B-0A7040929114}"/>
   </bookViews>
@@ -557,8 +557,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01EE5F85-A869-4E79-9B8B-E0ACF7B6DB8E}">
   <dimension ref="A1:B142"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A98" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B109" sqref="B109"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>